<commit_message>
test 75% of collect_tax_data
</commit_message>
<xml_diff>
--- a/tests/fixtures/test_expense_data.xlsx
+++ b/tests/fixtures/test_expense_data.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="240" yWindow="680" windowWidth="11720" windowHeight="8940" tabRatio="500"/>
+    <workbookView xWindow="7080" yWindow="23120" windowWidth="13560" windowHeight="5700" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Transactions" sheetId="1" r:id="rId1"/>
@@ -59,9 +59,6 @@
     <t>None: political</t>
   </si>
   <si>
-    <t>Another extra col</t>
-  </si>
-  <si>
     <t>Joe</t>
   </si>
   <si>
@@ -72,6 +69,9 @@
   </si>
   <si>
     <t>Arthur</t>
+  </si>
+  <si>
+    <t>Another extra</t>
   </si>
 </sst>
 </file>
@@ -118,12 +118,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="1" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -404,12 +405,12 @@
   <dimension ref="A1:G5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A5" sqref="A2:A5"/>
+      <selection sqref="A1:A1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="6.6640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="6.6640625" style="5" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="6.33203125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="12" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="7.6640625" style="1" bestFit="1" customWidth="1"/>
@@ -419,7 +420,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A1" s="2" t="s">
+      <c r="A1" s="4" t="s">
         <v>1</v>
       </c>
       <c r="B1" s="2" t="s">
@@ -438,15 +439,15 @@
         <v>5</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>10</v>
+        <v>14</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A2" s="4">
+      <c r="A2" s="5">
         <v>43101</v>
       </c>
       <c r="B2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>0</v>
@@ -462,11 +463,11 @@
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A3" s="4">
+      <c r="A3" s="5">
         <v>43132</v>
       </c>
       <c r="B3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C3" s="2" t="s">
         <v>0</v>
@@ -479,11 +480,11 @@
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A4" s="4">
+      <c r="A4" s="5">
         <v>43163</v>
       </c>
       <c r="B4" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C4" s="2" t="s">
         <v>0</v>
@@ -496,11 +497,11 @@
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A5" s="4">
+      <c r="A5" s="5">
         <v>43194</v>
       </c>
       <c r="B5" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C5" s="2" t="s">
         <v>0</v>

</xml_diff>

<commit_message>
track positive expenses and negative credits
</commit_message>
<xml_diff>
--- a/tests/fixtures/test_expense_data.xlsx
+++ b/tests/fixtures/test_expense_data.xlsx
@@ -9,10 +9,11 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="7080" yWindow="23120" windowWidth="13560" windowHeight="5700" tabRatio="500"/>
+    <workbookView xWindow="6300" yWindow="22220" windowWidth="19840" windowHeight="7020" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Transactions" sheetId="1" r:id="rId1"/>
+    <sheet name="Extra sheet" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="150000" concurrentCalc="0"/>
   <extLst>
@@ -27,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="16">
   <si>
     <t>Extra column</t>
   </si>
@@ -41,9 +42,6 @@
     <t>amount</t>
   </si>
   <si>
-    <t>tax_category</t>
-  </si>
-  <si>
     <t>spending_category</t>
   </si>
   <si>
@@ -72,14 +70,21 @@
   </si>
   <si>
     <t>Another extra</t>
+  </si>
+  <si>
+    <t>Tax category</t>
+  </si>
+  <si>
+    <t>Other</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <numFmts count="1">
+  <numFmts count="2">
     <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0.00"/>
+    <numFmt numFmtId="167" formatCode="m/d/yy;@"/>
   </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
@@ -118,13 +123,18 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="1" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="167" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="14" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -402,25 +412,25 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G5"/>
+  <dimension ref="A1:G7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:A1048576"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="130" workbookViewId="0">
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="6.6640625" style="5" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="6.6640625" style="8" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="6.33203125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="12" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="7.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8.33203125" style="1" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="29" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="18.33203125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="15.5" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="15.5" style="6" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A1" s="4" t="s">
+      <c r="A1" s="7" t="s">
         <v>1</v>
       </c>
       <c r="B1" s="2" t="s">
@@ -432,22 +442,22 @@
       <c r="D1" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="E1" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="F1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="G1" s="2" t="s">
-        <v>14</v>
+      <c r="G1" s="5" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A2" s="5">
+      <c r="A2" s="8">
         <v>43101</v>
       </c>
       <c r="B2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>0</v>
@@ -456,18 +466,21 @@
         <v>40</v>
       </c>
       <c r="E2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F2" t="s">
-        <v>6</v>
+        <v>5</v>
+      </c>
+      <c r="G2" s="6">
+        <v>43466</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A3" s="5">
+      <c r="A3" s="8">
         <v>43132</v>
       </c>
       <c r="B3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C3" s="2" t="s">
         <v>0</v>
@@ -476,15 +489,15 @@
         <v>60</v>
       </c>
       <c r="E3" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A4" s="5">
+      <c r="A4" s="8">
         <v>43163</v>
       </c>
       <c r="B4" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C4" s="2" t="s">
         <v>0</v>
@@ -493,15 +506,15 @@
         <v>80</v>
       </c>
       <c r="E4" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A5" s="5">
+      <c r="A5" s="8">
         <v>43194</v>
       </c>
       <c r="B5" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C5" s="2" t="s">
         <v>0</v>
@@ -510,10 +523,38 @@
         <v>100</v>
       </c>
       <c r="E5" t="s">
-        <v>8</v>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="D6" s="1">
+        <v>101</v>
+      </c>
+      <c r="E6" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="D7" s="1">
+        <v>-100</v>
+      </c>
+      <c r="E7" t="s">
+        <v>15</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>